<commit_message>
Add size summary analysis
</commit_message>
<xml_diff>
--- a/excel-data-summaries/density on pollen load.xlsx
+++ b/excel-data-summaries/density on pollen load.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire\Documents\Masters3\masters-thesis\excel-data-summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F6331-3B04-492A-867F-9BEB8B3FEDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B8AE17-6548-451F-A033-C845C0EC7274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{7A58EFC3-9473-4039-802C-AF122F4DB0FA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7A58EFC3-9473-4039-802C-AF122F4DB0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="raw data from r" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="103">
   <si>
     <t>Effects of local density on pollen load</t>
   </si>
@@ -256,12 +256,107 @@
   </si>
   <si>
     <t>Log (pollen) ~ Avg Dist + (1|Plant)</t>
+  </si>
+  <si>
+    <t>Plantago major</t>
+  </si>
+  <si>
+    <t>1, 25.71</t>
+  </si>
+  <si>
+    <t>1, 26.16</t>
+  </si>
+  <si>
+    <t>1, 28.02</t>
+  </si>
+  <si>
+    <t>1, 27.58</t>
+  </si>
+  <si>
+    <t>1, 67.92</t>
+  </si>
+  <si>
+    <t>4, 77.67</t>
+  </si>
+  <si>
+    <t>1, 73.07</t>
+  </si>
+  <si>
+    <t>3, 83.49</t>
+  </si>
+  <si>
+    <t>1, 28.76</t>
+  </si>
+  <si>
+    <t>2, 28.61</t>
+  </si>
+  <si>
+    <t>1, 15.28</t>
+  </si>
+  <si>
+    <t>3, 15.85</t>
+  </si>
+  <si>
+    <t>1, 77.29</t>
+  </si>
+  <si>
+    <t>1, 37.25</t>
+  </si>
+  <si>
+    <t>2, 15.26</t>
+  </si>
+  <si>
+    <t>1, 78.25</t>
+  </si>
+  <si>
+    <t>6, 81.76</t>
+  </si>
+  <si>
+    <t>1, 15.73</t>
+  </si>
+  <si>
+    <t>1, 23.72</t>
+  </si>
+  <si>
+    <t>1, 24.46</t>
+  </si>
+  <si>
+    <t>1, 13.24</t>
+  </si>
+  <si>
+    <t>1, 45.41</t>
+  </si>
+  <si>
+    <t>3, 39.19</t>
+  </si>
+  <si>
+    <t>1, 57.20</t>
+  </si>
+  <si>
+    <t>6, 78.43</t>
+  </si>
+  <si>
+    <t>1, 40.98</t>
+  </si>
+  <si>
+    <t>1, 26.55</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Avg dist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -328,26 +423,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDA198A-ABE1-4103-9EF5-EB76E2F5DED7}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="A3:F42"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,25 +1462,12 @@
     <col min="6" max="6" width="38.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1388,739 +1484,759 @@
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="13">
         <v>0.64790000000000003</v>
       </c>
-      <c r="E4" s="3">
-        <v>0.42820000000000003</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="13">
+        <v>0.43</v>
+      </c>
+      <c r="F4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
+        <v>75</v>
+      </c>
+      <c r="D5" s="14">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="14">
         <v>0.96750000000000003</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="15">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="15">
         <v>0.79769999999999996</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2">
+        <v>77</v>
+      </c>
+      <c r="D7" s="14">
         <v>26.626000000000001</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>1.8669999999999999E-5</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="15">
         <v>8.7058999999999997</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="18">
         <v>3.9090000000000001E-3</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="14">
         <v>2.5436999999999999</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="21">
         <v>1.2985E-2</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="15">
         <v>0.36470000000000002</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="15">
         <v>0.54790000000000005</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2">
+        <v>79</v>
+      </c>
+      <c r="D11" s="14">
         <v>10.7943</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="6">
         <v>5.2099999999999997E-7</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="15">
         <v>0.74890000000000001</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="15">
         <v>0.38965499999999997</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2">
+        <v>81</v>
+      </c>
+      <c r="D13" s="14">
         <v>5.53</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="17">
         <v>1.637E-3</v>
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14">
+        <v>82</v>
+      </c>
+      <c r="D14" s="13">
         <v>0.27629999999999999</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="13">
         <v>0.60319999999999996</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="2">
+        <v>83</v>
+      </c>
+      <c r="D15" s="14">
         <v>16.07</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="6">
         <v>2.0990000000000001E-5</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16">
+        <v>84</v>
+      </c>
+      <c r="D16" s="13">
         <v>3.0882999999999998</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="13">
         <v>9.8868999999999999E-2</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="2">
+        <v>85</v>
+      </c>
+      <c r="D17" s="14">
         <v>9.5165000000000006</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="22">
         <v>7.8299999999999995E-4</v>
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="13">
         <v>10.773</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="19">
         <v>1.1460000000000001E-3</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="14">
         <v>12.676</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="6">
         <v>1.4100000000000001E-9</v>
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20">
+        <v>86</v>
+      </c>
+      <c r="D20" s="13">
         <v>0.1053</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="13">
         <v>0.74639999999999995</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="14">
         <v>1.1213</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="14">
         <v>0.35210000000000002</v>
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22">
+        <v>87</v>
+      </c>
+      <c r="D22" s="13">
         <v>1.8782000000000001</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="13">
         <v>0.1787</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="2">
+        <v>88</v>
+      </c>
+      <c r="D23" s="14">
         <v>15.2418</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="7">
         <v>2.3000000000000001E-4</v>
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="13">
         <v>0.1067</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="13">
         <v>0.74429999999999996</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="14">
         <v>4.5964</v>
       </c>
-      <c r="E25" s="11">
-        <v>5.8810000000000004E-4</v>
+      <c r="E25" s="7">
+        <v>5.9000000000000003E-4</v>
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26">
+        <v>89</v>
+      </c>
+      <c r="D26" s="13">
         <v>0.1628</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="13">
         <v>0.68769999999999998</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="2">
+        <v>90</v>
+      </c>
+      <c r="D27" s="14">
         <v>7.9757999999999996</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="6">
         <v>8.7609999999999996E-7</v>
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
         <v>47</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="13">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="13">
         <v>0.85150000000000003</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="14">
         <v>5.9686000000000003</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="6">
         <v>1.8899999999999999E-6</v>
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
+      <c r="B30" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="2">
+        <v>91</v>
+      </c>
+      <c r="D30" s="14">
         <v>0.3498</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="14">
         <v>0.56259999999999999</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31">
+        <v>92</v>
+      </c>
+      <c r="D31" s="13">
         <v>0.94710000000000005</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="13">
         <v>0.34028000000000003</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="2">
+        <v>93</v>
+      </c>
+      <c r="D32" s="14">
         <v>3.2904</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="23">
         <v>8.1979999999999997E-2</v>
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="E33" s="24">
+        <v>5.8189999999999999E-2</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33">
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="13">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="E33">
+      <c r="E34" s="13">
         <v>0.92749999999999999</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F34" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="14">
         <v>0.63849999999999996</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E35" s="14">
         <v>0.59470000000000001</v>
       </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35">
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="13">
         <v>7.2263999999999999</v>
       </c>
-      <c r="E35" s="12">
-        <v>9.3900000000000008E-3</v>
-      </c>
-      <c r="F35" s="3" t="s">
+      <c r="E36" s="8">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="F36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" s="2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="14">
         <v>0.86099999999999999</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E37" s="14">
         <v>0.52739499999999995</v>
       </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
         <v>60</v>
       </c>
-      <c r="D37">
+      <c r="D38" s="13">
         <v>2.4367000000000001</v>
       </c>
-      <c r="E37">
+      <c r="E38" s="13">
         <v>0.1208</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="2" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D39" s="14">
         <v>11.7035</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E39" s="6">
         <v>1.581E-9</v>
       </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="s">
         <v>63</v>
       </c>
-      <c r="D39">
+      <c r="D40" s="13">
         <v>0.04</v>
       </c>
-      <c r="E39">
+      <c r="E40" s="13">
         <v>0.84189999999999998</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="2" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D41" s="14">
         <v>26.843</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E41" s="6">
         <v>3.1929999999999998E-16</v>
       </c>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" s="2">
+      <c r="B42" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="14">
         <v>1.3105</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E42" s="14">
         <v>0.25890000000000002</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F42" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="B43" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="14">
         <v>6.1580000000000004</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E43" s="21">
         <v>1.9720000000000001E-2</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F43" s="5" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>